<commit_message>
MTCloud Provider: Updated toolikit references and explicitly removed remaining unused thirdparty references for excel EPPlus etc...
</commit_message>
<xml_diff>
--- a/Sdl.MTCloud.Languages.Provider/Resources/DefaultMTLanguageCodes.xlsx
+++ b/Sdl.MTCloud.Languages.Provider/Resources/DefaultMTLanguageCodes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\VSTS\Sdl-Community\MTCloud.Languages.ExcelReader\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\VSTS\Sdl-Community\Sdl.MTCloud.Languages.Provider\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Languages" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Languages!$A$1:$D$610</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Languages!$A$1:$D$632</definedName>
     <definedName name="unifiedCodes" localSheetId="0">Languages!$A$2:$D$610</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2469" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2468" uniqueCount="1396">
   <si>
     <t>Language</t>
   </si>
@@ -4183,9 +4183,6 @@
   </si>
   <si>
     <t>sr-Latn-XK</t>
-  </si>
-  <si>
-    <t>g</t>
   </si>
   <si>
     <t>sw-CD</t>
@@ -4596,7 +4593,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A1:E632"/>
+      <selection pane="bottomLeft" activeCell="B210" sqref="B210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4619,10 +4616,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1394</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1395</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1396</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -13212,9 +13209,6 @@
       <c r="D627" t="s">
         <v>1091</v>
       </c>
-      <c r="E627" s="3" t="s">
-        <v>1385</v>
-      </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
@@ -13224,7 +13218,7 @@
         <v>241</v>
       </c>
       <c r="C628" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -13232,21 +13226,21 @@
         <v>197</v>
       </c>
       <c r="B629" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C629" t="s">
         <v>1387</v>
-      </c>
-      <c r="C629" t="s">
-        <v>1388</v>
       </c>
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="B630" t="s">
         <v>42</v>
       </c>
       <c r="C630" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.25">
@@ -13254,10 +13248,10 @@
         <v>221</v>
       </c>
       <c r="B631" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C631" t="s">
         <v>1391</v>
-      </c>
-      <c r="C631" t="s">
-        <v>1392</v>
       </c>
       <c r="D631" t="s">
         <v>206</v>
@@ -13271,17 +13265,17 @@
         <v>221</v>
       </c>
       <c r="B632" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C632" t="s">
         <v>1393</v>
-      </c>
-      <c r="C632" t="s">
-        <v>1394</v>
       </c>
       <c r="D632" t="s">
         <v>229</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D610"/>
+  <autoFilter ref="A1:D632"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>